<commit_message>
Setup table and user field updated
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>area_users</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>so,product,rate,quantity,_ref</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>name,value</t>
+  </si>
+  <si>
+    <t>name,code,phone,outstanding_normal,outstanding_overdue,outstanding_critical</t>
   </si>
 </sst>
 </file>
@@ -336,8 +345,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E24">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
     <filterColumn colId="3"/>
@@ -639,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,86 +698,86 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="1">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="1">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>38</v>
@@ -780,10 +789,10 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>38</v>
@@ -795,7 +804,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -810,10 +819,10 @@
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -825,42 +834,40 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="1">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -874,57 +881,57 @@
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="1">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
@@ -937,83 +944,100 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E20" s="4">
         <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1080</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1080</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="B24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1">
         <v>6</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
_ref field added to receipts table
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -183,9 +183,6 @@
     <t>fn_reserves</t>
   </si>
   <si>
-    <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date</t>
-  </si>
-  <si>
     <t>transaction,spt,price,tax,discount,total</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>fncode,user,store,start_num,end_num,quantity,current,progress,status</t>
+  </si>
+  <si>
+    <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>36</v>
@@ -868,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -932,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>36</v>
@@ -964,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>31</v>
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>31</v>
@@ -1060,7 +1060,7 @@
         <v>53</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>31</v>
@@ -1077,7 +1077,7 @@
         <v>54</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Fiscal year code field added
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -84,9 +84,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>format,digit_length</t>
-  </si>
-  <si>
     <t>pricelist,product,price</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>name,cocode,co_abr,brcode,br_abr</t>
   </si>
   <si>
-    <t>name,abr,start_date,end_date</t>
-  </si>
-  <si>
     <t>name,uom,narration,group1,group2,group3,group4</t>
   </si>
   <si>
@@ -202,6 +196,12 @@
   </si>
   <si>
     <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref</t>
+  </si>
+  <si>
+    <t>code,format,digit_length</t>
+  </si>
+  <si>
+    <t>code,name,abr,start_date,end_date</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -684,44 +684,44 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>24</v>
@@ -733,10 +733,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -751,7 +751,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
@@ -763,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
@@ -778,10 +778,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1">
         <v>18</v>
@@ -790,13 +790,13 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1">
         <v>24</v>
@@ -808,10 +808,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1">
         <v>24</v>
@@ -826,7 +826,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1">
         <v>24</v>
@@ -841,7 +841,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1">
         <v>24</v>
@@ -853,10 +853,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>24</v>
@@ -868,10 +868,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1">
         <v>12</v>
@@ -883,10 +883,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -900,10 +900,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -917,10 +917,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1">
         <v>24</v>
@@ -932,10 +932,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1">
         <v>12</v>
@@ -947,10 +947,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -964,10 +964,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -981,10 +981,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -998,10 +998,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
@@ -1015,10 +1015,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1">
         <v>12</v>
@@ -1030,10 +1030,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
@@ -1045,10 +1045,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1">
         <v>6</v>
@@ -1057,13 +1057,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="5">
         <v>3</v>
@@ -1074,13 +1074,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="5">
         <v>2</v>
@@ -1110,22 +1110,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transaction details price -> amount
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -180,9 +180,6 @@
     <t>fn_reserves</t>
   </si>
   <si>
-    <t>transaction,spt,price,tax,discount,total</t>
-  </si>
-  <si>
     <t>name,cocode,co_abr,brcode,br_abr</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>code,name,abr,start_date,end_date</t>
+  </si>
+  <si>
+    <t>transaction,spt,amount,tax,discount,total</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -868,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -932,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -964,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
@@ -1060,7 +1060,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
@@ -1077,7 +1077,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
backStack visible made false
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -192,9 +192,6 @@
     <t>fncode,user,store,start_num,end_num,quantity,current,progress,status</t>
   </si>
   <si>
-    <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref</t>
-  </si>
-  <si>
     <t>code,format,digit_length</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>transaction,spt,amount,tax,discount,total</t>
+  </si>
+  <si>
+    <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref,status</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
@@ -1060,7 +1060,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Sales order more fields added
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -159,12 +159,6 @@
     <t>store,product,direction,quantity,user,nature,date,type,_ref</t>
   </si>
   <si>
-    <t>docno,date,user,customer,fycode,fncode,progress,_ref</t>
-  </si>
-  <si>
-    <t>so,product,rate,quantity,_ref</t>
-  </si>
-  <si>
     <t>setup</t>
   </si>
   <si>
@@ -202,6 +196,12 @@
   </si>
   <si>
     <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref,status</t>
+  </si>
+  <si>
+    <t>docno,date,user,customer,fycode,fncode,payment_type,progress,_ref</t>
+  </si>
+  <si>
+    <t>so,product,rate,quantity,tax,discount,total,_ref</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -715,10 +715,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>35</v>
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -868,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -883,7 +883,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -900,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -932,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -964,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
@@ -1045,7 +1045,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>35</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
FYCode and FNCode added to receipt table
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -195,13 +195,13 @@
     <t>transaction,spt,amount,tax,discount,total</t>
   </si>
   <si>
-    <t>docno,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref,status</t>
-  </si>
-  <si>
     <t>docno,date,user,customer,fycode,fncode,payment_type,progress,_ref</t>
   </si>
   <si>
     <t>so,product,rate,quantity,tax,discount,total,_ref</t>
+  </si>
+  <si>
+    <t>docno,fycode,fncode,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref,status</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -883,7 +883,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -900,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -1060,7 +1060,7 @@
         <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Sales Order Sales added and Receipt fields added
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>area_users</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>docno,fycode,fncode,mode,customer,date,user,amount,bank,cheque,cheque_date,_ref,status</t>
+  </si>
+  <si>
+    <t>sales_order_sales</t>
+  </si>
+  <si>
+    <t>so,product,quantity,transaction,sale_quantity</t>
   </si>
 </sst>
 </file>
@@ -361,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E27">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
     <filterColumn colId="3"/>
@@ -664,9 +670,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -1087,6 +1093,23 @@
       </c>
       <c r="E26" s="5">
         <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload sync delay reduced to 1 minute for all user tables
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1">
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -979,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
@@ -1013,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="1">
-        <v>1080</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
@@ -1075,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1092,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="5">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Address and Email field in users table
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -165,9 +165,6 @@
     <t>name,value</t>
   </si>
   <si>
-    <t>name,code,phone,outstanding_normal,outstanding_overdue,outstanding_critical</t>
-  </si>
-  <si>
     <t>receipts</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>so,product,quantity,transaction,sale_quantity</t>
+  </si>
+  <si>
+    <t>name,code,email,phone,address,outstanding_normal,outstanding_overdue,outstanding_critical</t>
   </si>
 </sst>
 </file>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -784,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -889,7 +889,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -938,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -970,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -987,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
@@ -1051,22 +1051,24 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D24" s="1">
-        <v>6</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
@@ -1080,10 +1082,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -1097,10 +1099,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Currency added to store table
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -171,9 +171,6 @@
     <t>fn_reserves</t>
   </si>
   <si>
-    <t>name,cocode,co_abr,brcode,br_abr</t>
-  </si>
-  <si>
     <t>name,uom,narration,group1,group2,group3,group4</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>name,code,email,phone,address,outstanding_normal,outstanding_overdue,outstanding_critical</t>
+  </si>
+  <si>
+    <t>name,cocode,co_abr,brcode,br_abr,currency</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -784,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -874,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -889,7 +889,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -938,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -970,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -987,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
@@ -1051,7 +1051,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>30</v>
@@ -1068,7 +1068,7 @@
         <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
@@ -1085,7 +1085,7 @@
         <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Product Group table removed
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\Projects\epss\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="FindReplace" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>area_users</t>
   </si>
@@ -39,9 +44,6 @@
     <t>product_transaction_types</t>
   </si>
   <si>
-    <t>productgroups</t>
-  </si>
-  <si>
     <t>products</t>
   </si>
   <si>
@@ -85,9 +87,6 @@
   </si>
   <si>
     <t>pricelist,product,price</t>
-  </si>
-  <si>
-    <t>name,belongs,parent,tax1,tax2</t>
   </si>
   <si>
     <t>name,description,value</t>
@@ -213,8 +212,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,17 +362,20 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E27">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E26"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Table" dataDxfId="4"/>
     <tableColumn id="5" name="Fields" dataDxfId="3"/>
@@ -428,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,9 +462,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,6 +497,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,14 +673,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
@@ -685,214 +689,216 @@
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>24</v>
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1">
         <v>18</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1">
         <v>24</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1">
         <v>24</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1">
         <v>24</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1">
         <v>24</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -901,216 +907,199 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1">
         <v>12</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D22" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="5">
-        <v>3</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1124,33 +1113,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1159,12 +1148,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
outstanding and overdue renamed and removed critical
</commit_message>
<xml_diff>
--- a/SSAssetControllerDatabase.xlsx
+++ b/SSAssetControllerDatabase.xlsx
@@ -203,10 +203,10 @@
     <t>so,product,quantity,transaction,sale_quantity</t>
   </si>
   <si>
-    <t>name,code,email,phone,address,outstanding_normal,outstanding_overdue,outstanding_critical</t>
-  </si>
-  <si>
     <t>name,cocode,co_abr,brcode,br_abr,currency</t>
+  </si>
+  <si>
+    <t>name,code,email,phone,address,outstanding,overdue</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +927,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1040,7 +1040,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>28</v>

</xml_diff>